<commit_message>
Entra con usuario bueno
</commit_message>
<xml_diff>
--- a/Credenciales.xlsx
+++ b/Credenciales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18405"/>
   <workbookPr/>
-  <xr:revisionPtr documentId="8_{DF329193-4C8E-4B37-82F4-862E9AD1601C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21"/>
+  <xr:revisionPtr documentId="8_{704B8309-7335-4A8E-B452-B0796B25ECFF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21"/>
   <bookViews>
     <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>Usser</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>123456789abc1</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
   <si>
     <t>default</t>
@@ -84,9 +87,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -423,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -433,13 +439,16 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>23246383</v>
+      <c r="B4" s="2">
+        <v>12233</v>
       </c>
     </row>
     <row r="5" spans="1:3">

</xml_diff>

<commit_message>
Sigue en proceso ya que, solo funciona con  dos usuarios al llegar, al tercer usuario se sale y manda un null, que acaba con el proceso,
</commit_message>
<xml_diff>
--- a/Credenciales.xlsx
+++ b/Credenciales.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18405"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EA8075B-2AFA-4753-8558-A1FDEF4FD1C1}" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="8_{1C486A99-3C2A-42B5-85BB-D1B696243EB6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="171026"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
   <si>
     <t>Usser</t>
   </si>
@@ -39,12 +39,19 @@
   </si>
   <si>
     <t>123456789abc1</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -80,22 +87,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -112,10 +119,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -273,7 +280,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -282,13 +289,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -298,7 +305,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -307,7 +314,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -316,7 +323,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -326,12 +333,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -362,7 +369,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -381,7 +388,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -393,7 +400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
@@ -402,8 +409,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="28.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -424,6 +431,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
@@ -432,6 +442,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
@@ -440,6 +453,9 @@
       <c r="B4" s="2">
         <v>12233</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
@@ -459,12 +475,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{231D5409-E0AC-44FB-83C8-B6659F75EE31}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{DF08E155-93E6-4C0A-8A38-4F8413B46B02}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{C68685C7-CE11-40C1-A702-8D6863F63C3D}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{AAE203E9-4227-47EA-85BC-DCE143387A11}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{1E270BDA-5A0F-411B-B947-0FA3D080204B}"/>
+    <hyperlink r:id="rId1" ref="A4" xr:uid="{231D5409-E0AC-44FB-83C8-B6659F75EE31}"/>
+    <hyperlink r:id="rId2" ref="A3" xr:uid="{DF08E155-93E6-4C0A-8A38-4F8413B46B02}"/>
+    <hyperlink r:id="rId3" ref="A2" xr:uid="{C68685C7-CE11-40C1-A702-8D6863F63C3D}"/>
+    <hyperlink r:id="rId4" ref="A5" xr:uid="{AAE203E9-4227-47EA-85BC-DCE143387A11}"/>
+    <hyperlink r:id="rId5" ref="A6" xr:uid="{1E270BDA-5A0F-411B-B947-0FA3D080204B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>